<commit_message>
cleaning up graphs and tables
</commit_message>
<xml_diff>
--- a/resources/DM_Summary_Stats.xlsx
+++ b/resources/DM_Summary_Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Documents1\GitHub\Health_and_Avocados\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162967CF-8B96-4134-B801-5E51BDA0B0CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A903D58-FBC6-468D-AEB8-E088EEA26C8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="1155" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
+    <workbookView xWindow="6840" yWindow="9150" windowWidth="33285" windowHeight="19335" xr2:uid="{0C92DC33-7C36-430F-9CEF-FFE7D68A6C4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Final ML Models" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="55">
   <si>
     <t>Model</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Run Info</t>
+  </si>
+  <si>
+    <t>RMSE = 0.29</t>
   </si>
 </sst>
 </file>
@@ -320,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -352,9 +355,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -679,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E548DB6-46E4-4991-AEF9-13BA26A579B2}">
-  <dimension ref="B2:J8"/>
+  <dimension ref="B2:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -695,14 +695,13 @@
     <col min="7" max="7" width="5.7109375" customWidth="1"/>
     <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B2" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="25"/>
+      <c r="C2" s="24"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
         <v>21</v>
@@ -713,135 +712,221 @@
         <v>22</v>
       </c>
       <c r="I2" s="5"/>
-      <c r="J2" s="2"/>
-    </row>
-    <row r="3" spans="2:10" ht="26.25" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20" t="s">
+      <c r="D3" s="19"/>
+      <c r="E3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F3" s="20" t="s">
+      <c r="F3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20" t="s">
+      <c r="G3" s="19"/>
+      <c r="H3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="J3" s="2"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="17"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="18"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4"/>
+      <c r="H4" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="21">
-        <v>0.28999999999999998</v>
+        <v>39</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>43</v>
+      <c r="F5" s="20" t="s">
+        <v>40</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" s="4"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="I5" s="20" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" s="21" t="s">
-        <v>42</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C6" s="20"/>
       <c r="D6" s="4"/>
       <c r="E6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>40</v>
+      <c r="F6" s="20" t="s">
+        <v>46</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B11" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="2:9" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="G12" s="19"/>
+      <c r="H12" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="I12" s="19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="4"/>
+      <c r="H13" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I14" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="4"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="21" t="s">
+      <c r="C15" s="20"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I7" s="18" t="s">
+      <c r="G15" s="4"/>
+      <c r="H15" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="I15" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="J7" s="4"/>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C16" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="18" t="s">
+      <c r="D16" s="4"/>
+      <c r="E16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="F8" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="18" t="s">
+      <c r="G16" s="4"/>
+      <c r="H16" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="18" t="s">
+      <c r="I16" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="J8" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B11:C11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -886,10 +971,10 @@
         <v>20</v>
       </c>
       <c r="K2" s="5"/>
-      <c r="M2" s="22" t="s">
+      <c r="M2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="23"/>
+      <c r="N2" s="22"/>
     </row>
     <row r="3" spans="2:14" s="1" customFormat="1" ht="52.5" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">

</xml_diff>